<commit_message>
added week 2 and updated hours
</commit_message>
<xml_diff>
--- a/student-submissions/timelog.xlsx
+++ b/student-submissions/timelog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52640ecffeb77e34/Desktop/ap-csp_25-26/student-submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="11_F25DC773A252ABDACC104851519951F65BDE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1AAF957-64C6-4C33-A389-025F7DA1F009}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="11_F25DC773A252ABDACC104851519951F65BDE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32F52D04-4DE0-4B2A-B843-93B4F9FBC720}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -72,6 +72,21 @@
   </si>
   <si>
     <t>7:10pm</t>
+  </si>
+  <si>
+    <t>1:35pm</t>
+  </si>
+  <si>
+    <t>11:10am</t>
+  </si>
+  <si>
+    <t>week 2</t>
+  </si>
+  <si>
+    <t>week 1</t>
+  </si>
+  <si>
+    <t>10:00am</t>
   </si>
 </sst>
 </file>
@@ -121,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -133,13 +148,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -179,9 +192,13 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AE583CA1-19F4-4655-8238-5B4F7D02D2E6}" name="Table1" displayName="Table1" ref="A1:F5" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:F5" xr:uid="{AE583CA1-19F4-4655-8238-5B4F7D02D2E6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AE583CA1-19F4-4655-8238-5B4F7D02D2E6}" name="Table1" displayName="Table1" ref="A1:F6" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:F6" xr:uid="{AE583CA1-19F4-4655-8238-5B4F7D02D2E6}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{D7DFE132-8D06-4200-B59C-2AA5013F5117}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{4BBA18C6-2B58-4ABE-848F-D6FEBC7AB0AF}" name="Topics"/>
@@ -457,18 +474,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -494,22 +510,22 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+      <c r="A2" s="2">
         <v>45903</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2">
         <v>40</v>
       </c>
     </row>
@@ -534,14 +550,44 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="A4" s="2">
+        <v>45909</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="7"/>
+      <c r="A5" s="2">
+        <v>45911</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="6">
+        <v>2</v>
+      </c>
+      <c r="F5" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
week 3 2nd class
</commit_message>
<xml_diff>
--- a/student-submissions/timelog.xlsx
+++ b/student-submissions/timelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52640ecffeb77e34/Desktop/ap-csp_25-26/student-submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="11_F25DC773A252ABDACC104851519951F65BDE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A092502-3091-4F54-8F6C-42DDC3E8E877}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="11_F25DC773A252ABDACC104851519951F65BDE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41BA893C-757B-40B4-BA24-60E7E8AEF4D6}"/>
   <bookViews>
     <workbookView xWindow="45" yWindow="630" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t>3:45pm</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>9:30am</t>
+  </si>
+  <si>
+    <t>12:25pm</t>
   </si>
 </sst>
 </file>
@@ -224,8 +233,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AE583CA1-19F4-4655-8238-5B4F7D02D2E6}" name="Table1" displayName="Table1" ref="A1:F8" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:F8" xr:uid="{AE583CA1-19F4-4655-8238-5B4F7D02D2E6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AE583CA1-19F4-4655-8238-5B4F7D02D2E6}" name="Table1" displayName="Table1" ref="A1:F9" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:F9" xr:uid="{AE583CA1-19F4-4655-8238-5B4F7D02D2E6}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{D7DFE132-8D06-4200-B59C-2AA5013F5117}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{4BBA18C6-2B58-4ABE-848F-D6FEBC7AB0AF}" name="Topics"/>
@@ -501,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,6 +676,26 @@
         <v>15</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>45919</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>